<commit_message>
MultiPeriod HENS SP1 nearly complete
</commit_message>
<xml_diff>
--- a/Examples/MultiPeriodFlexibleHENSProblem/Floudas_Grossmann_1987/CompHENS_interface_FloudasGrossmann.xlsx
+++ b/Examples/MultiPeriodFlexibleHENSProblem/Floudas_Grossmann_1987/CompHENS_interface_FloudasGrossmann.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinashs\Desktop\CompHENS\Multiperiod\FloudasGrossmann1987\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA3B1B1-0189-4C49-A6C1-AA9C1EA8F26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E391C81B-022D-441B-A48A-07DA84520898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{91B6352A-F82C-47A0-9E88-BFB12B8F08AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="StreamDataPeriod1" sheetId="3" r:id="rId1"/>
-    <sheet name="StreamDataPeriod2" sheetId="1" r:id="rId2"/>
-    <sheet name="StreamDataPeriod3" sheetId="2" r:id="rId3"/>
+    <sheet name="Period_1" sheetId="3" r:id="rId1"/>
+    <sheet name="Period_2" sheetId="1" r:id="rId2"/>
+    <sheet name="Period_3" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -835,7 +835,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SP1 with multiperiod working properly
</commit_message>
<xml_diff>
--- a/Examples/MultiPeriodFlexibleHENSProblem/Floudas_Grossmann_1987/CompHENS_interface_FloudasGrossmann.xlsx
+++ b/Examples/MultiPeriodFlexibleHENSProblem/Floudas_Grossmann_1987/CompHENS_interface_FloudasGrossmann.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinashs\Desktop\CompHENS\Multiperiod\FloudasGrossmann1987\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E391C81B-022D-441B-A48A-07DA84520898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AA88CB-6248-4D98-A5A0-CBE09565BE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{91B6352A-F82C-47A0-9E88-BFB12B8F08AB}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C6" sqref="C6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,10 +604,10 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>650</v>
+        <v>380</v>
       </c>
       <c r="D6">
-        <v>649</v>
+        <v>379</v>
       </c>
       <c r="F6">
         <v>3.5</v>
@@ -624,10 +624,10 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>293</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>308</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>3.5</v>
@@ -647,7 +647,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C6" sqref="C6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,10 +792,10 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>650</v>
+        <v>380</v>
       </c>
       <c r="D6">
-        <v>649</v>
+        <v>379</v>
       </c>
       <c r="F6">
         <v>3.5</v>
@@ -812,10 +812,10 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>293</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>308</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>3.5</v>
@@ -835,7 +835,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,10 +980,10 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>650</v>
+        <v>380</v>
       </c>
       <c r="D6">
-        <v>649</v>
+        <v>379</v>
       </c>
       <c r="F6">
         <v>3.5</v>
@@ -1000,10 +1000,10 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>293</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>308</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>3.5</v>

</xml_diff>